<commit_message>
Add more information to L0 metadata template for L2130.
</commit_message>
<xml_diff>
--- a/metadata_templates/L0_metadata_template_PicarroL2130i.xlsx
+++ b/metadata_templates/L0_metadata_template_PicarroL2130i.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richf/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richfiorella/Documents/UU_vapor_processing_scripts/metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="6080" windowWidth="20660" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="27320" yWindow="3160" windowWidth="20660" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="L0_WBB_metadata.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Variable</t>
   </si>
@@ -195,16 +195,53 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>change in constant term of fitted baseline relative to empty cavity baseline; see Rev C 04-2015 manual</t>
+  </si>
+  <si>
+    <t>change in linear term of fitted baseline relative to empty cavity baseline; see Rev C 04-2015 manual</t>
+  </si>
+  <si>
+    <t>MRS residual of LS fit of measured spectra versus the expected spectra; see Rev C 04-2015 manual</t>
+  </si>
+  <si>
+    <t>Humidity; ppmv</t>
+  </si>
+  <si>
+    <t>Methane concentration in ppm</t>
+  </si>
+  <si>
+    <t>Relative value of degree of "openness" of cavity valve; continuously variable</t>
+  </si>
+  <si>
+    <t>Indicates which valves in vaporizer are activated; convert to binary to determine which valves are open</t>
+  </si>
+  <si>
+    <t>Temperature at warm box in instrument interior</t>
+  </si>
+  <si>
+    <t>Temperature sensor in the interior of the analyzer</t>
+  </si>
+  <si>
+    <t>Presumably code that states whether the instrument is operating as expected; not documented anywhere by Picarro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,8 +267,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +550,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,6 +711,9 @@
       <c r="A24" t="s">
         <v>31</v>
       </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -694,16 +735,25 @@
       <c r="A27" t="s">
         <v>34</v>
       </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -717,16 +767,25 @@
       <c r="A31" t="s">
         <v>38</v>
       </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -748,6 +807,9 @@
       <c r="A36" t="s">
         <v>43</v>
       </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -761,15 +823,24 @@
       <c r="A38" t="s">
         <v>45</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>